<commit_message>
Input/Expect parameters limit is upto 200.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoRestAutotestConstants.xlsx
+++ b/meta/program/BlancoRestAutotestConstants.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestAutotest/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2793F5-839F-5742-A510-675AC9F374DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D367ED29-5401-EB4D-B19E-84D240CD9B5B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10800" yWindow="5180" windowWidth="27320" windowHeight="14820" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -168,20 +168,6 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>inputのmax値(input1～input30)</t>
-    <rPh sb="9" eb="10">
-      <t>チ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>outputのmax値(output1～output30)</t>
-    <rPh sb="10" eb="11">
-      <t>チ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
     <t>TARGET_STYLE_BLANCO</t>
     <phoneticPr fontId="6"/>
   </si>
@@ -334,6 +320,20 @@
   </si>
   <si>
     <t>"/blancorestautotest"</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>inputのmax値(input1～input200)</t>
+    <rPh sb="9" eb="10">
+      <t>チ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>outputのmax値(output1～output200)</t>
+    <rPh sb="10" eb="11">
+      <t>チ</t>
+    </rPh>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -1145,7 +1145,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1189,7 +1189,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1216,8 +1216,8 @@
   </sheetPr>
   <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1264,7 +1264,7 @@
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="10"/>
@@ -1275,7 +1275,7 @@
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="10"/>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
@@ -1418,7 +1418,7 @@
         <v>22</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E20" s="27" t="s">
         <v>23</v>
@@ -1439,7 +1439,7 @@
         <v>22</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E21" s="29" t="s">
         <v>25</v>
@@ -1481,7 +1481,7 @@
         <v>22</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E23" s="26" t="s">
         <v>32</v>
@@ -1502,10 +1502,10 @@
         <v>33</v>
       </c>
       <c r="D24" s="26">
-        <v>30</v>
+        <v>200</v>
       </c>
       <c r="E24" s="26" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="F24" s="30"/>
       <c r="G24"/>
@@ -1523,10 +1523,10 @@
         <v>33</v>
       </c>
       <c r="D25" s="26">
-        <v>30</v>
+        <v>200</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="F25" s="30"/>
       <c r="G25"/>
@@ -1537,16 +1537,16 @@
         <v>7</v>
       </c>
       <c r="B26" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="39" t="s">
+      <c r="E26" s="39" t="s">
         <v>39</v>
-      </c>
-      <c r="D26" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="E26" s="39" t="s">
-        <v>41</v>
       </c>
       <c r="F26" s="30"/>
       <c r="G26"/>
@@ -1557,16 +1557,16 @@
         <v>8</v>
       </c>
       <c r="B27" s="38" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C27" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="E27" s="39" t="s">
         <v>39</v>
-      </c>
-      <c r="D27" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="E27" s="39" t="s">
-        <v>41</v>
       </c>
       <c r="F27" s="30"/>
       <c r="G27"/>
@@ -1577,16 +1577,16 @@
         <v>9</v>
       </c>
       <c r="B28" s="38" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C28" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" s="39" t="s">
         <v>39</v>
-      </c>
-      <c r="D28" s="39" t="s">
-        <v>45</v>
-      </c>
-      <c r="E28" s="39" t="s">
-        <v>41</v>
       </c>
       <c r="F28" s="30"/>
       <c r="G28"/>
@@ -1597,16 +1597,16 @@
         <v>10</v>
       </c>
       <c r="B29" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="E29" s="39" t="s">
         <v>46</v>
-      </c>
-      <c r="C29" s="39" t="s">
-        <v>39</v>
-      </c>
-      <c r="D29" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="E29" s="39" t="s">
-        <v>48</v>
       </c>
       <c r="F29" s="30"/>
       <c r="G29"/>
@@ -1617,16 +1617,16 @@
         <v>11</v>
       </c>
       <c r="B30" s="38" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C30" s="39" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D30" s="39" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E30" s="39" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F30" s="41"/>
       <c r="G30"/>
@@ -1650,7 +1650,7 @@
       </c>
       <c r="B32" s="25"/>
       <c r="C32" s="26" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D32" s="26"/>
       <c r="E32" s="26"/>
@@ -1663,16 +1663,16 @@
         <v>14</v>
       </c>
       <c r="B33" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="C33" s="26" t="s">
+      <c r="E33" s="26" t="s">
         <v>53</v>
-      </c>
-      <c r="D33" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="E33" s="26" t="s">
-        <v>55</v>
       </c>
       <c r="F33" s="30"/>
       <c r="G33"/>
@@ -1683,16 +1683,16 @@
         <v>15</v>
       </c>
       <c r="B34" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="C34" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="D34" s="26" t="s">
+      <c r="E34" s="26" t="s">
         <v>58</v>
-      </c>
-      <c r="E34" s="26" t="s">
-        <v>60</v>
       </c>
       <c r="F34" s="30"/>
       <c r="G34"/>
@@ -1703,16 +1703,16 @@
         <v>16</v>
       </c>
       <c r="B35" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="D35" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="C35" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="D35" s="26" t="s">
+      <c r="E35" s="26" t="s">
         <v>59</v>
-      </c>
-      <c r="E35" s="26" t="s">
-        <v>61</v>
       </c>
       <c r="F35" s="30"/>
       <c r="G35"/>

</xml_diff>